<commit_message>
minor tweaks to document
</commit_message>
<xml_diff>
--- a/Documents/Deliverable drafts_&_templates/Deliverable 2/SixGuys_Deliverable_2_SprintBackLog_3.xlsx
+++ b/Documents/Deliverable drafts_&_templates/Deliverable 2/SixGuys_Deliverable_2_SprintBackLog_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Desktop\Project-Burger\Documents\Deliverable drafts_&amp;_templates\Deliverable 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C778D0A-B3EC-4862-BAC4-AAB1CDF9019D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9329F5C-642E-492F-91FE-41F44323883E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4005" yWindow="885" windowWidth="21900" windowHeight="15180" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="420" windowWidth="21900" windowHeight="15180" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="76">
   <si>
     <t>Sprint Number</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>As a player I would like to start a new game so that I can begin the game.</t>
+  </si>
+  <si>
+    <t>As a player I want an environment to go through so that I can progress through the game</t>
   </si>
 </sst>
 </file>
@@ -302,7 +305,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +334,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -446,7 +461,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -480,16 +495,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="3" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="7" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in 20% - Accent4" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
@@ -1735,7 +1751,7 @@
   <dimension ref="A1:AMJ53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1773,133 +1789,145 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="17">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="18">
+        <v>3</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="18">
+        <v>5</v>
+      </c>
+      <c r="F2" s="18">
+        <v>3</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="18">
+        <v>1</v>
+      </c>
+      <c r="B3" s="18">
+        <v>3</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="18">
+        <v>13</v>
+      </c>
+      <c r="F3" s="18">
+        <v>3</v>
+      </c>
+      <c r="G3" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="18">
+        <v>3</v>
+      </c>
+      <c r="B4" s="18">
+        <v>3</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="18">
+        <v>5</v>
+      </c>
+      <c r="F4" s="18">
+        <v>3</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="11"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="18">
+        <v>1</v>
+      </c>
+      <c r="B5" s="18">
+        <v>3</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="18">
+        <v>5</v>
+      </c>
+      <c r="F5" s="18">
         <v>2</v>
       </c>
-      <c r="C2" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="D2" s="18" t="s">
+      <c r="G5" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="11"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="18">
+        <v>2</v>
+      </c>
+      <c r="B6" s="18">
+        <v>3</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="17">
-        <v>5</v>
-      </c>
-      <c r="F2" s="17">
+      <c r="E6" s="18">
+        <v>13</v>
+      </c>
+      <c r="F6" s="18">
+        <v>13</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="11"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="18">
+        <v>2</v>
+      </c>
+      <c r="B7" s="18">
         <v>3</v>
       </c>
-      <c r="G2" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="11"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="17">
-        <v>1</v>
-      </c>
-      <c r="B3" s="17">
-        <v>2</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" s="18" t="s">
+      <c r="C7" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E7" s="18">
         <v>13</v>
       </c>
-      <c r="F3" s="17">
-        <v>3</v>
-      </c>
-      <c r="G3" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="11"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" s="18"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="11"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
-        <v>1</v>
-      </c>
-      <c r="B5" s="17">
-        <v>2</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" s="17">
-        <v>5</v>
-      </c>
-      <c r="F5" s="17">
-        <v>2</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="H5" s="11"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
-        <v>2</v>
-      </c>
-      <c r="B6" s="17">
-        <v>3</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E6" s="17">
+      <c r="F7" s="18">
         <v>13</v>
       </c>
-      <c r="F6" s="17">
-        <v>13</v>
-      </c>
-      <c r="G6" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H6" s="11"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
-        <v>2</v>
-      </c>
-      <c r="B7" s="17">
-        <v>3</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="E7" s="17">
-        <v>13</v>
-      </c>
-      <c r="F7" s="17">
-        <v>13</v>
-      </c>
-      <c r="G7" s="19" t="s">
+      <c r="G7" s="20" t="s">
         <v>74</v>
       </c>
       <c r="H7" s="11"/>
@@ -1916,7 +1944,7 @@
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="10"/>
       <c r="B9" s="10"/>
-      <c r="C9" s="20"/>
+      <c r="C9" s="17"/>
       <c r="E9" s="9"/>
       <c r="F9" s="10"/>
       <c r="G9" s="7"/>
@@ -1925,7 +1953,7 @@
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
       <c r="B10" s="10"/>
-      <c r="C10" s="20"/>
+      <c r="C10" s="17"/>
       <c r="E10" s="9"/>
       <c r="F10" s="10"/>
       <c r="G10" s="7"/>
@@ -1934,7 +1962,7 @@
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
       <c r="B11" s="10"/>
-      <c r="C11" s="20"/>
+      <c r="C11" s="17"/>
       <c r="E11" s="9"/>
       <c r="F11" s="10"/>
       <c r="G11" s="7"/>
@@ -1943,7 +1971,7 @@
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="10"/>
       <c r="B12" s="10"/>
-      <c r="C12" s="20"/>
+      <c r="C12" s="17"/>
       <c r="E12" s="9"/>
       <c r="F12" s="10"/>
       <c r="G12" s="7"/>
@@ -1952,7 +1980,7 @@
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
-      <c r="C13" s="20"/>
+      <c r="C13" s="17"/>
       <c r="E13" s="9"/>
       <c r="F13" s="10"/>
       <c r="G13" s="7"/>
@@ -1961,7 +1989,7 @@
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
-      <c r="C14" s="20"/>
+      <c r="C14" s="17"/>
       <c r="E14" s="9"/>
       <c r="F14" s="10"/>
       <c r="G14" s="7"/>
@@ -1970,7 +1998,7 @@
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
-      <c r="C15" s="20"/>
+      <c r="C15" s="17"/>
       <c r="E15" s="9"/>
       <c r="F15" s="10"/>
       <c r="G15" s="7"/>
@@ -1979,7 +2007,7 @@
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
-      <c r="C16" s="20"/>
+      <c r="C16" s="17"/>
       <c r="E16" s="9"/>
       <c r="F16" s="10"/>
       <c r="G16" s="7"/>
@@ -1988,7 +2016,7 @@
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
-      <c r="C17" s="20"/>
+      <c r="C17" s="17"/>
       <c r="E17" s="9"/>
       <c r="F17" s="10"/>
       <c r="G17" s="7"/>
@@ -1997,7 +2025,7 @@
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
-      <c r="C18" s="20"/>
+      <c r="C18" s="17"/>
       <c r="E18" s="9"/>
       <c r="F18" s="10"/>
       <c r="G18" s="7"/>
@@ -2006,7 +2034,7 @@
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
-      <c r="C19" s="20"/>
+      <c r="C19" s="17"/>
       <c r="E19" s="9"/>
       <c r="F19" s="10"/>
       <c r="G19" s="7"/>
@@ -2015,7 +2043,7 @@
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="10"/>
       <c r="B20" s="10"/>
-      <c r="C20" s="20"/>
+      <c r="C20" s="17"/>
       <c r="E20" s="9"/>
       <c r="F20" s="10"/>
       <c r="G20" s="7"/>
@@ -2024,7 +2052,7 @@
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="10"/>
       <c r="B21" s="10"/>
-      <c r="C21" s="20"/>
+      <c r="C21" s="17"/>
       <c r="E21" s="9"/>
       <c r="F21" s="10"/>
       <c r="G21" s="7"/>
@@ -2033,7 +2061,7 @@
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="10"/>
       <c r="B22" s="10"/>
-      <c r="C22" s="20"/>
+      <c r="C22" s="17"/>
       <c r="E22" s="9"/>
       <c r="F22" s="10"/>
       <c r="G22" s="7"/>
@@ -2042,7 +2070,7 @@
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="10"/>
-      <c r="C23" s="20"/>
+      <c r="C23" s="17"/>
       <c r="E23" s="9"/>
       <c r="F23" s="10"/>
       <c r="G23" s="7"/>
@@ -2051,7 +2079,7 @@
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="10"/>
-      <c r="C24" s="20"/>
+      <c r="C24" s="17"/>
       <c r="E24" s="9"/>
       <c r="F24" s="10"/>
       <c r="G24" s="7"/>
@@ -2060,7 +2088,7 @@
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="10"/>
       <c r="B25" s="10"/>
-      <c r="C25" s="20"/>
+      <c r="C25" s="17"/>
       <c r="E25" s="9"/>
       <c r="F25" s="10"/>
       <c r="G25" s="12"/>

</xml_diff>